<commit_message>
se modifican datos principales de enero 2023
</commit_message>
<xml_diff>
--- a/Data/2023/1. Enero 2023/calculos_finales_Enero2023.xlsx
+++ b/Data/2023/1. Enero 2023/calculos_finales_Enero2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\QuantCo_Streamlit\Data\2023\1. Enero 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025C8B20-1F38-43CC-9948-DFC3E482AAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B4E96E-E0FD-4E4A-88DA-B483602A11DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="total" sheetId="1" r:id="rId1"/>
@@ -549,7 +549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H296"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,6 +862,9 @@
       </c>
       <c r="C2" s="1">
         <v>10339.129999999999</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
         <v>-0.18627250506907489</v>

</xml_diff>

<commit_message>
se modifica linea de código No 908 para filtrar datos negativos
</commit_message>
<xml_diff>
--- a/Data/2023/1. Enero 2023/calculos_finales_Enero2023.xlsx
+++ b/Data/2023/1. Enero 2023/calculos_finales_Enero2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\QuantCo_Streamlit\Data\2023\1. Enero 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B4E96E-E0FD-4E4A-88DA-B483602A11DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A1D861-5D73-4E09-905B-31DA3F3784EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -819,13 +819,14 @@
   <dimension ref="A1:H296"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
se sube archivo de quantstats para terminar resultados de enero2023
</commit_message>
<xml_diff>
--- a/Data/2023/1. Enero 2023/calculos_finales_Enero2023.xlsx
+++ b/Data/2023/1. Enero 2023/calculos_finales_Enero2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Documents\QuantCo_Streamlit\Data\2023\1. Enero 2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FEA565-CAE8-4E94-9758-E79C158B5DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3A8581-2304-4458-B580-494B662F1706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DeepAtlas!$A$1:$H$238</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -90,7 +101,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
-    <numFmt numFmtId="170" formatCode="0.000000000000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -256,7 +267,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,10 +829,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H296"/>
+  <dimension ref="A1:J296"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="D162" sqref="D162"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,6 +841,7 @@
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.5546875" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -858,16 +870,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="B2" s="6">
-        <v>44928.032685185193</v>
+        <v>44936.740949074083</v>
       </c>
       <c r="C2" s="1">
-        <v>10339.129999999999</v>
+        <v>8516.0000000000091</v>
       </c>
       <c r="D2" s="12">
-        <v>0</v>
+        <v>-4.5789979674295662E-2</v>
       </c>
       <c r="E2">
         <v>-0.18627250506907489</v>
@@ -884,16 +896,16 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
-        <v>1</v>
+        <v>68</v>
       </c>
       <c r="B3" s="6">
-        <v>44928.032685185193</v>
+        <v>44935.497997685183</v>
       </c>
       <c r="C3" s="1">
-        <v>10337.6</v>
+        <v>9015.7700000000077</v>
       </c>
       <c r="D3" s="12">
-        <v>-1.4798150327932641E-4</v>
+        <v>-3.709047799595222E-2</v>
       </c>
       <c r="E3">
         <v>-0.18627250506907489</v>
@@ -910,16 +922,16 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="B4" s="6">
-        <v>44928.388865740737</v>
+        <v>44932.85833333333</v>
       </c>
       <c r="C4" s="1">
-        <v>10340.290000000001</v>
+        <v>9335.2800000000079</v>
       </c>
       <c r="D4" s="12">
-        <v>2.6021513697571658E-4</v>
+        <v>-2.7662105269736229E-2</v>
       </c>
       <c r="E4">
         <v>-0.18627250506907489</v>
@@ -936,16 +948,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="11">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="B5" s="6">
-        <v>44928.414560185192</v>
+        <v>44935.633379629631</v>
       </c>
       <c r="C5" s="1">
-        <v>10350.56</v>
+        <v>8766.9800000000068</v>
       </c>
       <c r="D5" s="12">
-        <v>9.9320231831034889E-4</v>
+        <v>-2.759498079476308E-2</v>
       </c>
       <c r="E5">
         <v>-0.18627250506907489</v>
@@ -962,16 +974,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="B6" s="6">
-        <v>44929.410416666673</v>
+        <v>44932.814074074071</v>
       </c>
       <c r="C6" s="1">
-        <v>10336.219999999999</v>
+        <v>9600.8600000000079</v>
       </c>
       <c r="D6" s="12">
-        <v>-1.385432285789356E-3</v>
+        <v>-2.35834329155119E-2</v>
       </c>
       <c r="E6">
         <v>-0.18627250506907489</v>
@@ -988,16 +1000,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="B7" s="6">
-        <v>44929.420277777783</v>
+        <v>44932.776030092587</v>
       </c>
       <c r="C7" s="1">
-        <v>10323.76</v>
+        <v>9832.7500000000073</v>
       </c>
       <c r="D7" s="12">
-        <v>-1.205469697819761E-3</v>
+        <v>-1.9068445483739319E-2</v>
       </c>
       <c r="E7">
         <v>-0.18627250506907489</v>
@@ -1014,16 +1026,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="B8" s="6">
-        <v>44929.427997685183</v>
+        <v>44936.613854166673</v>
       </c>
       <c r="C8" s="1">
-        <v>10306.950000000001</v>
+        <v>8817.6300000000083</v>
       </c>
       <c r="D8" s="12">
-        <v>-1.628282718699303E-3</v>
+        <v>-1.540930118819106E-2</v>
       </c>
       <c r="E8">
         <v>-0.18627250506907489</v>
@@ -1040,16 +1052,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="11">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="B9" s="6">
-        <v>44929.438113425917</v>
+        <v>44932.74291666667</v>
       </c>
       <c r="C9" s="1">
-        <v>10305.99</v>
+        <v>10023.89000000001</v>
       </c>
       <c r="D9" s="12">
-        <v>-9.3141035902855052E-5</v>
+        <v>-1.3288853408197189E-2</v>
       </c>
       <c r="E9">
         <v>-0.18627250506907489</v>
@@ -1066,16 +1078,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
-        <v>8</v>
+        <v>154</v>
       </c>
       <c r="B10" s="6">
-        <v>44929.459849537037</v>
+        <v>44957.365972222222</v>
       </c>
       <c r="C10" s="1">
-        <v>10318.93</v>
+        <v>10803.01</v>
       </c>
       <c r="D10" s="12">
-        <v>1.255580492509845E-3</v>
+        <v>-1.2518327306498491E-2</v>
       </c>
       <c r="E10">
         <v>-0.18627250506907489</v>
@@ -1092,16 +1104,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="B11" s="6">
-        <v>44929.461782407408</v>
+        <v>44932.74013888889</v>
       </c>
       <c r="C11" s="1">
-        <v>10333.540000000001</v>
+        <v>10158.89000000001</v>
       </c>
       <c r="D11" s="12">
-        <v>1.4158444722467409E-3</v>
+        <v>-9.1778105703800295E-3</v>
       </c>
       <c r="E11">
         <v>-0.18627250506907489</v>
@@ -1118,16 +1130,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="B12" s="6">
-        <v>44929.517858796287</v>
+        <v>44932.719861111109</v>
       </c>
       <c r="C12" s="1">
-        <v>10347.84</v>
+        <v>10252.990000000011</v>
       </c>
       <c r="D12" s="12">
-        <v>1.383843290876152E-3</v>
+        <v>-6.3295310273978611E-3</v>
       </c>
       <c r="E12">
         <v>-0.18627250506907489</v>
@@ -1144,16 +1156,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="B13" s="6">
-        <v>44929.555300925917</v>
+        <v>44932.715856481482</v>
       </c>
       <c r="C13" s="1">
-        <v>10366.299999999999</v>
+        <v>10318.30000000001</v>
       </c>
       <c r="D13" s="12">
-        <v>1.7839471812473029E-3</v>
+        <v>-6.1806102016186406E-3</v>
       </c>
       <c r="E13">
         <v>-0.18627250506907489</v>
@@ -1170,16 +1182,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B14" s="6">
-        <v>44937.018784722219</v>
+        <v>44936.834733796299</v>
       </c>
       <c r="C14" s="1">
-        <v>10365.83</v>
+        <v>8605.4300000000076</v>
       </c>
       <c r="D14" s="12">
-        <v>-4.5339224216900398E-5</v>
+        <v>-5.8950194421276692E-3</v>
       </c>
       <c r="E14">
         <v>-0.18627250506907489</v>
@@ -1196,16 +1208,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="11">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="B15" s="6">
-        <v>44937.147349537037</v>
+        <v>44932.712060185193</v>
       </c>
       <c r="C15" s="1">
-        <v>10371.129999999999</v>
+        <v>10382.47000000001</v>
       </c>
       <c r="D15" s="12">
-        <v>5.112952846033636E-4</v>
+        <v>-5.3981197108485812E-3</v>
       </c>
       <c r="E15">
         <v>-0.18627250506907489</v>
@@ -1222,16 +1234,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="11">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="B16" s="6">
-        <v>44944.195844907408</v>
+        <v>44932.709722222222</v>
       </c>
       <c r="C16" s="1">
-        <v>10373.459999999999</v>
+        <v>10438.820000000011</v>
       </c>
       <c r="D16" s="12">
-        <v>2.2466211492866431E-4</v>
+        <v>-2.5417040118791419E-3</v>
       </c>
       <c r="E16">
         <v>-0.18627250506907489</v>
@@ -1248,16 +1260,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B17" s="6">
-        <v>44951.512499999997</v>
+        <v>44929.427997685183</v>
       </c>
       <c r="C17" s="1">
-        <v>10375.69</v>
+        <v>10306.950000000001</v>
       </c>
       <c r="D17" s="12">
-        <v>2.1497166808370771E-4</v>
+        <v>-1.628282718699303E-3</v>
       </c>
       <c r="E17">
         <v>-0.18627250506907489</v>
@@ -1274,16 +1286,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="B18" s="6">
-        <v>44957.425000000003</v>
+        <v>44944.280578703707</v>
       </c>
       <c r="C18" s="1">
-        <v>10377.6</v>
+        <v>10801.400000000011</v>
       </c>
       <c r="D18" s="12">
-        <v>1.8408414283777039E-4</v>
+        <v>-1.6055429591349531E-3</v>
       </c>
       <c r="E18">
         <v>-0.18627250506907489</v>
@@ -1300,68 +1312,68 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="11">
-        <v>17</v>
+        <v>102</v>
       </c>
       <c r="B19" s="6">
-        <v>44925.76458333333</v>
+        <v>44944.375439814823</v>
       </c>
       <c r="C19" s="1">
-        <v>10377.23</v>
+        <v>10785.160000000011</v>
       </c>
       <c r="D19" s="12">
-        <v>-3.565371569547171E-5</v>
+        <v>-1.5035088044141891E-3</v>
       </c>
       <c r="E19">
         <v>-0.18627250506907489</v>
       </c>
       <c r="F19" s="2">
-        <v>4.6060746222620352E-4</v>
+        <v>4.4385392570033273E-2</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H19" s="5">
-        <v>1.8424298489048141E-3</v>
+        <v>0.17754157028013309</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="11">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B20" s="6">
-        <v>44925.796932870369</v>
+        <v>44929.410416666673</v>
       </c>
       <c r="C20" s="1">
-        <v>10382.379999999999</v>
+        <v>10336.219999999999</v>
       </c>
       <c r="D20" s="12">
-        <v>4.9627887210745847E-4</v>
+        <v>-1.385432285789356E-3</v>
       </c>
       <c r="E20">
         <v>-0.18627250506907489</v>
       </c>
       <c r="F20" s="2">
-        <v>4.6060746222620352E-4</v>
+        <v>4.4385392570033273E-2</v>
       </c>
       <c r="G20" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H20" s="5">
-        <v>1.8424298489048141E-3</v>
+        <v>0.17754157028013309</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="11">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B21" s="6">
-        <v>44928.440983796303</v>
+        <v>44929.852106481478</v>
       </c>
       <c r="C21" s="1">
-        <v>10384.25</v>
+        <v>10397.75</v>
       </c>
       <c r="D21" s="12">
-        <v>1.8011284503183231E-4</v>
+        <v>-1.3043482436921881E-3</v>
       </c>
       <c r="E21">
         <v>-0.18627250506907489</v>
@@ -1378,16 +1390,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B22" s="6">
-        <v>44928.760416666657</v>
+        <v>44929.420277777783</v>
       </c>
       <c r="C22" s="1">
-        <v>10386.120000000001</v>
+        <v>10323.76</v>
       </c>
       <c r="D22" s="12">
-        <v>1.8008041023676041E-4</v>
+        <v>-1.205469697819761E-3</v>
       </c>
       <c r="E22">
         <v>-0.18627250506907489</v>
@@ -1404,16 +1416,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="11">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B23" s="6">
-        <v>44928.793749999997</v>
+        <v>44930.245416666658</v>
       </c>
       <c r="C23" s="1">
-        <v>10386.11</v>
+        <v>10385.290000000001</v>
       </c>
       <c r="D23" s="12">
-        <v>-9.6282346051523859E-7</v>
+        <v>-1.1983361785000699E-3</v>
       </c>
       <c r="E23">
         <v>-0.18627250506907489</v>
@@ -1430,16 +1442,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="B24" s="6">
-        <v>44929.044699074067</v>
+        <v>44944.388553240737</v>
       </c>
       <c r="C24" s="1">
-        <v>10391.950000000001</v>
+        <v>10773.510000000009</v>
       </c>
       <c r="D24" s="12">
-        <v>5.6228944234182343E-4</v>
+        <v>-1.0801879619773971E-3</v>
       </c>
       <c r="E24">
         <v>-0.18627250506907489</v>
@@ -1456,16 +1468,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B25" s="6">
-        <v>44929.071597222217</v>
+        <v>44929.569444444453</v>
       </c>
       <c r="C25" s="1">
-        <v>10393.780000000001</v>
+        <v>10394.27</v>
       </c>
       <c r="D25" s="12">
-        <v>1.7609784496652739E-4</v>
+        <v>-7.8251097582193729E-4</v>
       </c>
       <c r="E25">
         <v>-0.18627250506907489</v>
@@ -1482,16 +1494,16 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="11">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B26" s="6">
-        <v>44929.136805555558</v>
+        <v>44930.397650462961</v>
       </c>
       <c r="C26" s="1">
-        <v>10395.75</v>
+        <v>10379.400000000011</v>
       </c>
       <c r="D26" s="12">
-        <v>1.895364342905381E-4</v>
+        <v>-5.6714834154847349E-4</v>
       </c>
       <c r="E26">
         <v>-0.18627250506907489</v>
@@ -1508,16 +1520,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="B27" s="6">
-        <v>44929.166666666657</v>
+        <v>44945.1875</v>
       </c>
       <c r="C27" s="1">
-        <v>10395.36</v>
+        <v>10840.71000000001</v>
       </c>
       <c r="D27" s="12">
-        <v>-3.751533078411029E-5</v>
+        <v>-2.867993013532244E-4</v>
       </c>
       <c r="E27">
         <v>-0.18627250506907489</v>
@@ -1534,16 +1546,16 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="11">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="B28" s="6">
-        <v>44929.258506944447</v>
+        <v>44949.086111111108</v>
       </c>
       <c r="C28" s="1">
-        <v>10400.51</v>
+        <v>10859.100000000009</v>
       </c>
       <c r="D28" s="12">
-        <v>4.9541333825864342E-4</v>
+        <v>-2.7895081351458911E-4</v>
       </c>
       <c r="E28">
         <v>-0.18627250506907489</v>
@@ -1560,16 +1572,16 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="11">
-        <v>27</v>
+        <v>149</v>
       </c>
       <c r="B29" s="6">
-        <v>44929.488194444442</v>
+        <v>44956.417372685188</v>
       </c>
       <c r="C29" s="1">
-        <v>10402.41</v>
+        <v>10924.78</v>
       </c>
       <c r="D29" s="12">
-        <v>1.8268334918181139E-4</v>
+        <v>-2.7361483632981631E-4</v>
       </c>
       <c r="E29">
         <v>-0.18627250506907489</v>
@@ -1586,16 +1598,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="11">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="B30" s="6">
-        <v>44929.569444444453</v>
+        <v>44951.617361111108</v>
       </c>
       <c r="C30" s="1">
-        <v>10394.27</v>
+        <v>10892.41</v>
       </c>
       <c r="D30" s="12">
-        <v>-7.8251097582193729E-4</v>
+        <v>-2.7075746005644769E-4</v>
       </c>
       <c r="E30">
         <v>-0.18627250506907489</v>
@@ -1612,16 +1624,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
-        <v>29</v>
+        <v>118</v>
       </c>
       <c r="B31" s="6">
-        <v>44929.63726851852</v>
+        <v>44945.773622685178</v>
       </c>
       <c r="C31" s="1">
-        <v>10393.870000000001</v>
+        <v>10850.660000000011</v>
       </c>
       <c r="D31" s="12">
-        <v>-3.8482740971623741E-5</v>
+        <v>-2.6811454664221751E-4</v>
       </c>
       <c r="E31">
         <v>-0.18627250506907489</v>
@@ -1638,16 +1650,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="11">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B32" s="6">
-        <v>44929.67564814815</v>
+        <v>44938.798622685194</v>
       </c>
       <c r="C32" s="1">
-        <v>10400.9</v>
+        <v>10778.77000000001</v>
       </c>
       <c r="D32" s="12">
-        <v>6.7636020077221914E-4</v>
+        <v>-2.6804777742939212E-4</v>
       </c>
       <c r="E32">
         <v>-0.18627250506907489</v>
@@ -1664,16 +1676,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="11">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="B33" s="6">
-        <v>44929.695497685178</v>
+        <v>44950.740300925929</v>
       </c>
       <c r="C33" s="1">
-        <v>10409.290000000001</v>
+        <v>10882</v>
       </c>
       <c r="D33" s="12">
-        <v>8.0666096203207971E-4</v>
+        <v>-2.5081007980898301E-4</v>
       </c>
       <c r="E33">
         <v>-0.18627250506907489</v>
@@ -1690,16 +1702,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="B34" s="6">
-        <v>44929.790277777778</v>
+        <v>44944.630555555559</v>
       </c>
       <c r="C34" s="1">
-        <v>10411.33</v>
+        <v>10830.77000000001</v>
       </c>
       <c r="D34" s="12">
-        <v>1.959787843359706E-4</v>
+        <v>-2.5015045950138592E-4</v>
       </c>
       <c r="E34">
         <v>-0.18627250506907489</v>
@@ -1716,16 +1728,16 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
-        <v>33</v>
+        <v>97</v>
       </c>
       <c r="B35" s="6">
-        <v>44929.852106481478</v>
+        <v>44943.533333333333</v>
       </c>
       <c r="C35" s="1">
-        <v>10397.75</v>
+        <v>10805.47000000001</v>
       </c>
       <c r="D35" s="12">
-        <v>-1.3043482436921881E-3</v>
+        <v>-2.3778594453760521E-4</v>
       </c>
       <c r="E35">
         <v>-0.18627250506907489</v>
@@ -1742,16 +1754,16 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="11">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B36" s="6">
-        <v>44930.245416666658</v>
+        <v>44928.032685185193</v>
       </c>
       <c r="C36" s="1">
-        <v>10385.290000000001</v>
+        <v>10337.6</v>
       </c>
       <c r="D36" s="12">
-        <v>-1.1983361785000699E-3</v>
+        <v>-1.4798150327932641E-4</v>
       </c>
       <c r="E36">
         <v>-0.18627250506907489</v>
@@ -1768,16 +1780,16 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="11">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B37" s="6">
-        <v>44930.397650462961</v>
+        <v>44929.438113425917</v>
       </c>
       <c r="C37" s="1">
-        <v>10379.400000000011</v>
+        <v>10305.99</v>
       </c>
       <c r="D37" s="12">
-        <v>-5.6714834154847349E-4</v>
+        <v>-9.3141035902855052E-5</v>
       </c>
       <c r="E37">
         <v>-0.18627250506907489</v>
@@ -1794,16 +1806,16 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="11">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="B38" s="6">
-        <v>44930.421134259261</v>
+        <v>44944.406585648147</v>
       </c>
       <c r="C38" s="1">
-        <v>10381.69000000001</v>
+        <v>10772.64</v>
       </c>
       <c r="D38" s="12">
-        <v>2.2062932346766931E-4</v>
+        <v>-8.0753626255591904E-5</v>
       </c>
       <c r="E38">
         <v>-0.18627250506907489</v>
@@ -1820,16 +1832,16 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B39" s="6">
-        <v>44930.427187499998</v>
+        <v>44932.618750000001</v>
       </c>
       <c r="C39" s="1">
-        <v>10394.79000000001</v>
+        <v>10457.27000000001</v>
       </c>
       <c r="D39" s="12">
-        <v>1.2618369456225409E-3</v>
+        <v>-5.3548393882829608E-5</v>
       </c>
       <c r="E39">
         <v>-0.18627250506907489</v>
@@ -1846,16 +1858,16 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B40" s="6">
-        <v>44930.43822916667</v>
+        <v>44937.018784722219</v>
       </c>
       <c r="C40" s="1">
-        <v>10408.400000000011</v>
+        <v>10365.83</v>
       </c>
       <c r="D40" s="12">
-        <v>1.309309759985666E-3</v>
+        <v>-4.5339224216900398E-5</v>
       </c>
       <c r="E40">
         <v>-0.18627250506907489</v>
@@ -1872,16 +1884,16 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
-        <v>39</v>
+        <v>141</v>
       </c>
       <c r="B41" s="6">
-        <v>44930.47928240741</v>
+        <v>44952.828472222223</v>
       </c>
       <c r="C41" s="1">
-        <v>10427.420000000009</v>
+        <v>10910.34</v>
       </c>
       <c r="D41" s="12">
-        <v>1.827370200991441E-3</v>
+        <v>-4.307654518764803E-5</v>
       </c>
       <c r="E41">
         <v>-0.18627250506907489</v>
@@ -1898,16 +1910,16 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="11">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B42" s="6">
-        <v>44930.644456018519</v>
+        <v>44929.63726851852</v>
       </c>
       <c r="C42" s="1">
-        <v>10428.500000000009</v>
+        <v>10393.870000000001</v>
       </c>
       <c r="D42" s="12">
-        <v>1.035730794385348E-4</v>
+        <v>-3.8482740971623741E-5</v>
       </c>
       <c r="E42">
         <v>-0.18627250506907489</v>
@@ -1924,16 +1936,16 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
-        <v>41</v>
+        <v>138</v>
       </c>
       <c r="B43" s="6">
-        <v>44930.783333333333</v>
+        <v>44951.787546296298</v>
       </c>
       <c r="C43" s="1">
-        <v>10430.38000000001</v>
+        <v>10903.91</v>
       </c>
       <c r="D43" s="12">
-        <v>1.8027520736429989E-4</v>
+        <v>-3.7599776969154952E-5</v>
       </c>
       <c r="E43">
         <v>-0.18627250506907489</v>
@@ -1950,16 +1962,16 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="11">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B44" s="6">
-        <v>44930.93472222222</v>
+        <v>44929.166666666657</v>
       </c>
       <c r="C44" s="1">
-        <v>10430.02000000001</v>
+        <v>10395.36</v>
       </c>
       <c r="D44" s="12">
-        <v>-3.4514562269105653E-5</v>
+        <v>-3.751533078411029E-5</v>
       </c>
       <c r="E44">
         <v>-0.18627250506907489</v>
@@ -1976,16 +1988,16 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="11">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="B45" s="6">
-        <v>44931.104166666657</v>
+        <v>44943.226388888892</v>
       </c>
       <c r="C45" s="1">
-        <v>10435.14000000001</v>
+        <v>10802.98000000001</v>
       </c>
       <c r="D45" s="12">
-        <v>4.9089071737173917E-4</v>
+        <v>-3.609984662189536E-5</v>
       </c>
       <c r="E45">
         <v>-0.18627250506907489</v>
@@ -2002,16 +2014,16 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="11">
-        <v>44</v>
+        <v>143</v>
       </c>
       <c r="B46" s="6">
-        <v>44931.324305555558</v>
+        <v>44953.313888888893</v>
       </c>
       <c r="C46" s="1">
-        <v>10437.14000000001</v>
+        <v>10915.070000000011</v>
       </c>
       <c r="D46" s="12">
-        <v>1.9166010230819991E-4</v>
+        <v>-3.572914013694195E-5</v>
       </c>
       <c r="E46">
         <v>-0.18627250506907489</v>
@@ -2028,42 +2040,42 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="11">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B47" s="6">
-        <v>44931.417361111111</v>
+        <v>44925.76458333333</v>
       </c>
       <c r="C47" s="1">
-        <v>10436.78000000001</v>
+        <v>10377.23</v>
       </c>
       <c r="D47" s="12">
-        <v>-3.4492207635516969E-5</v>
+        <v>-3.565371569547171E-5</v>
       </c>
       <c r="E47">
         <v>-0.18627250506907489</v>
       </c>
       <c r="F47" s="2">
-        <v>4.4385392570033273E-2</v>
+        <v>4.6060746222620352E-4</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H47" s="5">
-        <v>0.17754157028013309</v>
+        <v>1.8424298489048141E-3</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="11">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B48" s="6">
-        <v>44931.434976851851</v>
+        <v>44930.93472222222</v>
       </c>
       <c r="C48" s="1">
-        <v>10441.87000000001</v>
+        <v>10430.02000000001</v>
       </c>
       <c r="D48" s="12">
-        <v>4.8769831308126399E-4</v>
+        <v>-3.4514562269105653E-5</v>
       </c>
       <c r="E48">
         <v>-0.18627250506907489</v>
@@ -2078,18 +2090,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="11">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B49" s="6">
-        <v>44931.480555555558</v>
+        <v>44931.417361111111</v>
       </c>
       <c r="C49" s="1">
-        <v>10443.79000000001</v>
+        <v>10436.78000000001</v>
       </c>
       <c r="D49" s="12">
-        <v>1.8387511049255961E-4</v>
+        <v>-3.4492207635516969E-5</v>
       </c>
       <c r="E49">
         <v>-0.18627250506907489</v>
@@ -2104,18 +2116,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" s="11">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="B50" s="6">
-        <v>44931.597222222219</v>
+        <v>44949.918749999997</v>
       </c>
       <c r="C50" s="1">
-        <v>10445.73000000001</v>
+        <v>10875.84</v>
       </c>
       <c r="D50" s="12">
-        <v>1.857563202631862E-4</v>
+        <v>-3.4019203380641898E-5</v>
       </c>
       <c r="E50">
         <v>-0.18627250506907489</v>
@@ -2130,18 +2142,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" s="11">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="B51" s="6">
-        <v>44931.714629629627</v>
+        <v>44942.468055555553</v>
       </c>
       <c r="C51" s="1">
-        <v>10448.19000000001</v>
+        <v>10796.06000000001</v>
       </c>
       <c r="D51" s="12">
-        <v>2.3550292799057179E-4</v>
+        <v>-2.500849825826101E-5</v>
       </c>
       <c r="E51">
         <v>-0.18627250506907489</v>
@@ -2156,18 +2168,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="11">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="B52" s="6">
-        <v>44931.809039351851</v>
+        <v>44928.793749999997</v>
       </c>
       <c r="C52" s="1">
-        <v>10450.010000000009</v>
+        <v>10386.11</v>
       </c>
       <c r="D52" s="12">
-        <v>1.741928506275858E-4</v>
+        <v>-9.6282346051523859E-7</v>
       </c>
       <c r="E52">
         <v>-0.18627250506907489</v>
@@ -2182,18 +2194,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" s="11">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="B53" s="6">
-        <v>44932.020486111112</v>
+        <v>44928.032685185193</v>
       </c>
       <c r="C53" s="1">
-        <v>10452.05000000001</v>
+        <v>10339.129999999999</v>
       </c>
       <c r="D53" s="12">
-        <v>1.952151241961797E-4</v>
+        <v>0</v>
       </c>
       <c r="E53">
         <v>-0.18627250506907489</v>
@@ -2207,19 +2219,20 @@
       <c r="H53" s="5">
         <v>0.17754157028013309</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J53" s="12"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" s="11">
-        <v>52</v>
+        <v>115</v>
       </c>
       <c r="B54" s="6">
-        <v>44932.340277777781</v>
+        <v>44945.403217592589</v>
       </c>
       <c r="C54" s="1">
-        <v>10453.990000000011</v>
+        <v>10841.750000000009</v>
       </c>
       <c r="D54" s="12">
-        <v>1.8560952157709029E-4</v>
+        <v>9.593467586532789E-5</v>
       </c>
       <c r="E54">
         <v>-0.18627250506907489</v>
@@ -2234,18 +2247,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="11">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="B55" s="6">
-        <v>44932.42291666667</v>
+        <v>44943.862500000003</v>
       </c>
       <c r="C55" s="1">
-        <v>10455.930000000009</v>
+        <v>10818.77000000001</v>
       </c>
       <c r="D55" s="12">
-        <v>1.8557507707583909E-4</v>
+        <v>9.7062967057581773E-5</v>
       </c>
       <c r="E55">
         <v>-0.18627250506907489</v>
@@ -2260,18 +2273,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B56" s="6">
-        <v>44932.530555555553</v>
+        <v>44930.644456018519</v>
       </c>
       <c r="C56" s="1">
-        <v>10457.830000000011</v>
+        <v>10428.500000000009</v>
       </c>
       <c r="D56" s="12">
-        <v>1.8171506503961149E-4</v>
+        <v>1.035730794385348E-4</v>
       </c>
       <c r="E56">
         <v>-0.18627250506907489</v>
@@ -2286,18 +2299,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" s="11">
-        <v>55</v>
+        <v>110</v>
       </c>
       <c r="B57" s="6">
-        <v>44932.618750000001</v>
+        <v>44944.645914351851</v>
       </c>
       <c r="C57" s="1">
-        <v>10457.27000000001</v>
+        <v>10831.930000000009</v>
       </c>
       <c r="D57" s="12">
-        <v>-5.3548393882829608E-5</v>
+        <v>1.071022651206732E-4</v>
       </c>
       <c r="E57">
         <v>-0.18627250506907489</v>
@@ -2312,18 +2325,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" s="11">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="B58" s="6">
-        <v>44932.645925925928</v>
+        <v>44949.135416666657</v>
       </c>
       <c r="C58" s="1">
-        <v>10463.500000000009</v>
+        <v>10860.350000000009</v>
       </c>
       <c r="D58" s="12">
-        <v>5.9575778381915079E-4</v>
+        <v>1.151108287058555E-4</v>
       </c>
       <c r="E58">
         <v>-0.18627250506907489</v>
@@ -2338,18 +2351,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="11">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B59" s="6">
-        <v>44932.661111111112</v>
+        <v>44938.831608796303</v>
       </c>
       <c r="C59" s="1">
-        <v>10465.420000000009</v>
+        <v>10780.170000000009</v>
       </c>
       <c r="D59" s="12">
-        <v>1.834950064509844E-4</v>
+        <v>1.298849497670673E-4</v>
       </c>
       <c r="E59">
         <v>-0.18627250506907489</v>
@@ -2364,18 +2377,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="11">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="B60" s="6">
-        <v>44932.709722222222</v>
+        <v>44945.797488425917</v>
       </c>
       <c r="C60" s="1">
-        <v>10438.820000000011</v>
+        <v>10852.30000000001</v>
       </c>
       <c r="D60" s="12">
-        <v>-2.5417040118791419E-3</v>
+        <v>1.5114287978801319E-4</v>
       </c>
       <c r="E60">
         <v>-0.18627250506907489</v>
@@ -2390,18 +2403,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="11">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="B61" s="6">
-        <v>44932.712060185193</v>
+        <v>44943.598460648151</v>
       </c>
       <c r="C61" s="1">
-        <v>10382.47000000001</v>
+        <v>10807.170000000009</v>
       </c>
       <c r="D61" s="12">
-        <v>-5.3981197108485812E-3</v>
+        <v>1.573277238289261E-4</v>
       </c>
       <c r="E61">
         <v>-0.18627250506907489</v>
@@ -2416,18 +2429,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" s="11">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="B62" s="6">
-        <v>44932.715856481482</v>
+        <v>44956.475578703707</v>
       </c>
       <c r="C62" s="1">
-        <v>10318.30000000001</v>
+        <v>10926.51</v>
       </c>
       <c r="D62" s="12">
-        <v>-6.1806102016186406E-3</v>
+        <v>1.5835559160004559E-4</v>
       </c>
       <c r="E62">
         <v>-0.18627250506907489</v>
@@ -2442,18 +2455,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="11">
-        <v>61</v>
+        <v>136</v>
       </c>
       <c r="B63" s="6">
-        <v>44932.719861111109</v>
+        <v>44951.695104166669</v>
       </c>
       <c r="C63" s="1">
-        <v>10252.990000000011</v>
+        <v>10894.17</v>
       </c>
       <c r="D63" s="12">
-        <v>-6.3295310273978611E-3</v>
+        <v>1.615804032348844E-4</v>
       </c>
       <c r="E63">
         <v>-0.18627250506907489</v>
@@ -2468,18 +2481,18 @@
         <v>0.17754157028013309</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="11">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="B64" s="6">
-        <v>44932.74013888889</v>
+        <v>44951.082870370366</v>
       </c>
       <c r="C64" s="1">
-        <v>10158.89000000001</v>
+        <v>10883.76</v>
       </c>
       <c r="D64" s="12">
-        <v>-9.1778105703800295E-3</v>
+        <v>1.6173497518834351E-4</v>
       </c>
       <c r="E64">
         <v>-0.18627250506907489</v>
@@ -2496,16 +2509,16 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="11">
-        <v>63</v>
+        <v>140</v>
       </c>
       <c r="B65" s="6">
-        <v>44932.74291666667</v>
+        <v>44952.524305555547</v>
       </c>
       <c r="C65" s="1">
-        <v>10023.89000000001</v>
+        <v>10910.81</v>
       </c>
       <c r="D65" s="12">
-        <v>-1.3288853408197189E-2</v>
+        <v>1.6591804931698209E-4</v>
       </c>
       <c r="E65">
         <v>-0.18627250506907489</v>
@@ -2522,16 +2535,16 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="11">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="B66" s="6">
-        <v>44932.776030092587</v>
+        <v>44949.615972222222</v>
       </c>
       <c r="C66" s="1">
-        <v>9832.7500000000073</v>
+        <v>10872.31</v>
       </c>
       <c r="D66" s="12">
-        <v>-1.9068445483739319E-2</v>
+        <v>1.665056805113529E-4</v>
       </c>
       <c r="E66">
         <v>-0.18627250506907489</v>
@@ -2548,16 +2561,16 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="11">
-        <v>65</v>
+        <v>129</v>
       </c>
       <c r="B67" s="6">
-        <v>44932.814074074071</v>
+        <v>44950.526400462957</v>
       </c>
       <c r="C67" s="1">
-        <v>9600.8600000000079</v>
+        <v>10882.76</v>
       </c>
       <c r="D67" s="12">
-        <v>-2.35834329155119E-2</v>
+        <v>1.6818415337649381E-4</v>
       </c>
       <c r="E67">
         <v>-0.18627250506907489</v>
@@ -2574,16 +2587,16 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="11">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="B68" s="6">
-        <v>44932.85833333333</v>
+        <v>44951.480567129627</v>
       </c>
       <c r="C68" s="1">
-        <v>9335.2800000000079</v>
+        <v>10895.36</v>
       </c>
       <c r="D68" s="12">
-        <v>-2.7662105269736229E-2</v>
+        <v>1.6982588715674929E-4</v>
       </c>
       <c r="E68">
         <v>-0.18627250506907489</v>
@@ -2600,16 +2613,16 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="11">
-        <v>67</v>
+        <v>126</v>
       </c>
       <c r="B69" s="6">
-        <v>44935.151863425926</v>
+        <v>44949.729884259257</v>
       </c>
       <c r="C69" s="1">
-        <v>9363.0500000000084</v>
+        <v>10876.21</v>
       </c>
       <c r="D69" s="12">
-        <v>2.9747366977745941E-3</v>
+        <v>1.7012495448009979E-4</v>
       </c>
       <c r="E69">
         <v>-0.18627250506907489</v>
@@ -2626,16 +2639,16 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="11">
-        <v>68</v>
+        <v>153</v>
       </c>
       <c r="B70" s="6">
-        <v>44935.497997685183</v>
+        <v>44956.916678240741</v>
       </c>
       <c r="C70" s="1">
-        <v>9015.7700000000077</v>
+        <v>10939.96</v>
       </c>
       <c r="D70" s="12">
-        <v>-3.709047799595222E-2</v>
+        <v>1.7096220638168619E-4</v>
       </c>
       <c r="E70">
         <v>-0.18627250506907489</v>
@@ -2652,16 +2665,16 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="11">
-        <v>69</v>
+        <v>148</v>
       </c>
       <c r="B71" s="6">
-        <v>44935.633379629631</v>
+        <v>44956.379166666673</v>
       </c>
       <c r="C71" s="1">
-        <v>8766.9800000000068</v>
+        <v>10927.77</v>
       </c>
       <c r="D71" s="12">
-        <v>-2.759498079476308E-2</v>
+        <v>1.7115294849867621E-4</v>
       </c>
       <c r="E71">
         <v>-0.18627250506907489</v>
@@ -2678,16 +2691,16 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="11">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="B72" s="6">
-        <v>44935.720451388886</v>
+        <v>44944.789629629631</v>
       </c>
       <c r="C72" s="1">
-        <v>8823.2700000000077</v>
+        <v>10841.910000000011</v>
       </c>
       <c r="D72" s="12">
-        <v>6.42068306303889E-3</v>
+        <v>1.72508588529352E-4</v>
       </c>
       <c r="E72">
         <v>-0.18627250506907489</v>
@@ -2704,16 +2717,16 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="11">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="B73" s="6">
-        <v>44935.72420138889</v>
+        <v>44956.059178240743</v>
       </c>
       <c r="C73" s="1">
-        <v>8887.7700000000077</v>
+        <v>10925.9</v>
       </c>
       <c r="D73" s="12">
-        <v>7.3102149203185807E-3</v>
+        <v>1.7301338977171449E-4</v>
       </c>
       <c r="E73">
         <v>-0.18627250506907489</v>
@@ -2730,16 +2743,16 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="11">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="B74" s="6">
-        <v>44936.094629629632</v>
+        <v>44953.647245370368</v>
       </c>
       <c r="C74" s="1">
-        <v>8955.6300000000083</v>
+        <v>10922.02</v>
       </c>
       <c r="D74" s="12">
-        <v>7.6352110821951147E-3</v>
+        <v>1.7307486266182609E-4</v>
       </c>
       <c r="E74">
         <v>-0.18627250506907489</v>
@@ -2756,16 +2769,16 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="11">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B75" s="6">
-        <v>44936.613854166673</v>
+        <v>44931.809039351851</v>
       </c>
       <c r="C75" s="1">
-        <v>8817.6300000000083</v>
+        <v>10450.010000000009</v>
       </c>
       <c r="D75" s="12">
-        <v>-1.540930118819106E-2</v>
+        <v>1.741928506275858E-4</v>
       </c>
       <c r="E75">
         <v>-0.18627250506907489</v>
@@ -2782,16 +2795,16 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="11">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="B76" s="6">
-        <v>44936.667129629634</v>
+        <v>44956.690983796303</v>
       </c>
       <c r="C76" s="1">
-        <v>8924.6600000000089</v>
+        <v>10938.09</v>
       </c>
       <c r="D76" s="12">
-        <v>1.213818225532259E-2</v>
+        <v>1.7464964914615239E-4</v>
       </c>
       <c r="E76">
         <v>-0.18627250506907489</v>
@@ -2808,16 +2821,16 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="11">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B77" s="6">
-        <v>44936.740949074083</v>
+        <v>44929.071597222217</v>
       </c>
       <c r="C77" s="1">
-        <v>8516.0000000000091</v>
+        <v>10393.780000000001</v>
       </c>
       <c r="D77" s="12">
-        <v>-4.5789979674295662E-2</v>
+        <v>1.7609784496652739E-4</v>
       </c>
       <c r="E77">
         <v>-0.18627250506907489</v>
@@ -2834,16 +2847,16 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="11">
-        <v>76</v>
+        <v>113</v>
       </c>
       <c r="B78" s="6">
-        <v>44936.818287037036</v>
+        <v>44944.915972222218</v>
       </c>
       <c r="C78" s="1">
-        <v>8656.4600000000082</v>
+        <v>10843.820000000011</v>
       </c>
       <c r="D78" s="12">
-        <v>1.6493658994833241E-2</v>
+        <v>1.7616822128196929E-4</v>
       </c>
       <c r="E78">
         <v>-0.18627250506907489</v>
@@ -2860,16 +2873,16 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="11">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B79" s="6">
-        <v>44936.834733796299</v>
+        <v>44942.167546296303</v>
       </c>
       <c r="C79" s="1">
-        <v>8605.4300000000076</v>
+        <v>10794.400000000011</v>
       </c>
       <c r="D79" s="12">
-        <v>-5.8950194421276692E-3</v>
+        <v>1.7697491496404541E-4</v>
       </c>
       <c r="E79">
         <v>-0.18627250506907489</v>
@@ -2886,16 +2899,16 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="11">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B80" s="6">
-        <v>44937.317881944437</v>
+        <v>44942.301412037043</v>
       </c>
       <c r="C80" s="1">
-        <v>8803.6700000000073</v>
+        <v>10796.330000000011</v>
       </c>
       <c r="D80" s="12">
-        <v>2.3036617577506299E-2</v>
+        <v>1.787964129549291E-4</v>
       </c>
       <c r="E80">
         <v>-0.18627250506907489</v>
@@ -2912,16 +2925,16 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="11">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B81" s="6">
-        <v>44937.421574074076</v>
+        <v>44939.059050925927</v>
       </c>
       <c r="C81" s="1">
-        <v>9043.9000000000069</v>
+        <v>10792.490000000011</v>
       </c>
       <c r="D81" s="12">
-        <v>2.7287483515397559E-2</v>
+        <v>1.7886004062805941E-4</v>
       </c>
       <c r="E81">
         <v>-0.18627250506907489</v>
@@ -2938,16 +2951,16 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="11">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="B82" s="6">
-        <v>44937.444606481477</v>
+        <v>44928.760416666657</v>
       </c>
       <c r="C82" s="1">
-        <v>9303.1300000000065</v>
+        <v>10386.120000000001</v>
       </c>
       <c r="D82" s="12">
-        <v>2.8663519057043899E-2</v>
+        <v>1.8008041023676041E-4</v>
       </c>
       <c r="E82">
         <v>-0.18627250506907489</v>
@@ -2964,16 +2977,16 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="11">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="B83" s="6">
-        <v>44937.47047453704</v>
+        <v>44928.440983796303</v>
       </c>
       <c r="C83" s="1">
-        <v>9413.820000000007</v>
+        <v>10384.25</v>
       </c>
       <c r="D83" s="12">
-        <v>1.189814610781537E-2</v>
+        <v>1.8011284503183231E-4</v>
       </c>
       <c r="E83">
         <v>-0.18627250506907489</v>
@@ -2990,16 +3003,16 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="11">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="B84" s="6">
-        <v>44937.472256944442</v>
+        <v>44930.783333333333</v>
       </c>
       <c r="C84" s="1">
-        <v>9690.8700000000063</v>
+        <v>10430.38000000001</v>
       </c>
       <c r="D84" s="12">
-        <v>2.9430135694117791E-2</v>
+        <v>1.8027520736429989E-4</v>
       </c>
       <c r="E84">
         <v>-0.18627250506907489</v>
@@ -3016,16 +3029,16 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="11">
-        <v>83</v>
+        <v>130</v>
       </c>
       <c r="B85" s="6">
-        <v>44937.573206018518</v>
+        <v>44950.554907407408</v>
       </c>
       <c r="C85" s="1">
-        <v>10023.55000000001</v>
+        <v>10884.73</v>
       </c>
       <c r="D85" s="12">
-        <v>3.4329219151634449E-2</v>
+        <v>1.810202558909513E-4</v>
       </c>
       <c r="E85">
         <v>-0.18627250506907489</v>
@@ -3042,16 +3055,16 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="11">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="B86" s="6">
-        <v>44937.678206018521</v>
+        <v>44932.530555555553</v>
       </c>
       <c r="C86" s="1">
-        <v>10388.330000000011</v>
+        <v>10457.830000000011</v>
       </c>
       <c r="D86" s="12">
-        <v>3.6392296142584213E-2</v>
+        <v>1.8171506503961149E-4</v>
       </c>
       <c r="E86">
         <v>-0.18627250506907489</v>
@@ -3068,16 +3081,16 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="11">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="B87" s="6">
-        <v>44937.700902777768</v>
+        <v>44953.696539351848</v>
       </c>
       <c r="C87" s="1">
-        <v>10781.660000000011</v>
+        <v>10924.01</v>
       </c>
       <c r="D87" s="12">
-        <v>3.7862678601854112E-2</v>
+        <v>1.822007284366656E-4</v>
       </c>
       <c r="E87">
         <v>-0.18627250506907489</v>
@@ -3094,16 +3107,16 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="11">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="B88" s="6">
-        <v>44938.798622685194</v>
+        <v>44929.488194444442</v>
       </c>
       <c r="C88" s="1">
-        <v>10778.77000000001</v>
+        <v>10402.41</v>
       </c>
       <c r="D88" s="12">
-        <v>-2.6804777742939212E-4</v>
+        <v>1.8268334918181139E-4</v>
       </c>
       <c r="E88">
         <v>-0.18627250506907489</v>
@@ -3120,16 +3133,16 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="11">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="B89" s="6">
-        <v>44938.831608796303</v>
+        <v>44945.688194444447</v>
       </c>
       <c r="C89" s="1">
-        <v>10780.170000000009</v>
+        <v>10853.570000000011</v>
       </c>
       <c r="D89" s="12">
-        <v>1.298849497670673E-4</v>
+        <v>1.8338343356449899E-4</v>
       </c>
       <c r="E89">
         <v>-0.18627250506907489</v>
@@ -3146,16 +3159,16 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="11">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B90" s="6">
-        <v>44938.836238425924</v>
+        <v>44932.661111111112</v>
       </c>
       <c r="C90" s="1">
-        <v>10790.56000000001</v>
+        <v>10465.420000000009</v>
       </c>
       <c r="D90" s="12">
-        <v>9.6380669321538548E-4</v>
+        <v>1.834950064509844E-4</v>
       </c>
       <c r="E90">
         <v>-0.18627250506907489</v>
@@ -3172,16 +3185,16 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="11">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="B91" s="6">
-        <v>44939.059050925927</v>
+        <v>44931.480555555558</v>
       </c>
       <c r="C91" s="1">
-        <v>10792.490000000011</v>
+        <v>10443.79000000001</v>
       </c>
       <c r="D91" s="12">
-        <v>1.7886004062805941E-4</v>
+        <v>1.8387511049255961E-4</v>
       </c>
       <c r="E91">
         <v>-0.18627250506907489</v>
@@ -3198,16 +3211,16 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="11">
-        <v>90</v>
+        <v>16</v>
       </c>
       <c r="B92" s="6">
-        <v>44942.167546296303</v>
+        <v>44957.425000000003</v>
       </c>
       <c r="C92" s="1">
-        <v>10794.400000000011</v>
+        <v>10377.6</v>
       </c>
       <c r="D92" s="12">
-        <v>1.7697491496404541E-4</v>
+        <v>1.8408414283777039E-4</v>
       </c>
       <c r="E92">
         <v>-0.18627250506907489</v>
@@ -3224,16 +3237,16 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="11">
-        <v>91</v>
+        <v>53</v>
       </c>
       <c r="B93" s="6">
-        <v>44942.301412037043</v>
+        <v>44932.42291666667</v>
       </c>
       <c r="C93" s="1">
-        <v>10796.330000000011</v>
+        <v>10455.930000000009</v>
       </c>
       <c r="D93" s="12">
-        <v>1.787964129549291E-4</v>
+        <v>1.8557507707583909E-4</v>
       </c>
       <c r="E93">
         <v>-0.18627250506907489</v>
@@ -3250,16 +3263,16 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="11">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="B94" s="6">
-        <v>44942.468055555553</v>
+        <v>44932.340277777781</v>
       </c>
       <c r="C94" s="1">
-        <v>10796.06000000001</v>
+        <v>10453.990000000011</v>
       </c>
       <c r="D94" s="12">
-        <v>-2.500849825826101E-5</v>
+        <v>1.8560952157709029E-4</v>
       </c>
       <c r="E94">
         <v>-0.18627250506907489</v>
@@ -3276,16 +3289,16 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="11">
-        <v>93</v>
+        <v>48</v>
       </c>
       <c r="B95" s="6">
-        <v>44942.51085648148</v>
+        <v>44931.597222222219</v>
       </c>
       <c r="C95" s="1">
-        <v>10801.36000000001</v>
+        <v>10445.73000000001</v>
       </c>
       <c r="D95" s="12">
-        <v>4.9091983556959207E-4</v>
+        <v>1.857563202631862E-4</v>
       </c>
       <c r="E95">
         <v>-0.18627250506907489</v>
@@ -3328,16 +3341,16 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97" s="11">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="B97" s="6">
-        <v>44943.226388888892</v>
+        <v>44949.700023148151</v>
       </c>
       <c r="C97" s="1">
-        <v>10802.98000000001</v>
+        <v>10874.36</v>
       </c>
       <c r="D97" s="12">
-        <v>-3.609984662189536E-5</v>
+        <v>1.8855238675130609E-4</v>
       </c>
       <c r="E97">
         <v>-0.18627250506907489</v>
@@ -3354,16 +3367,16 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98" s="11">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="B98" s="6">
-        <v>44943.428611111107</v>
+        <v>44929.136805555558</v>
       </c>
       <c r="C98" s="1">
-        <v>10808.04000000001</v>
+        <v>10395.75</v>
       </c>
       <c r="D98" s="12">
-        <v>4.6838927777326228E-4</v>
+        <v>1.895364342905381E-4</v>
       </c>
       <c r="E98">
         <v>-0.18627250506907489</v>
@@ -3380,16 +3393,16 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99" s="11">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="B99" s="6">
-        <v>44943.533333333333</v>
+        <v>44931.324305555558</v>
       </c>
       <c r="C99" s="1">
-        <v>10805.47000000001</v>
+        <v>10437.14000000001</v>
       </c>
       <c r="D99" s="12">
-        <v>-2.3778594453760521E-4</v>
+        <v>1.9166010230819991E-4</v>
       </c>
       <c r="E99">
         <v>-0.18627250506907489</v>
@@ -3406,16 +3419,16 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100" s="11">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="B100" s="6">
-        <v>44943.598460648151</v>
+        <v>44932.020486111112</v>
       </c>
       <c r="C100" s="1">
-        <v>10807.170000000009</v>
+        <v>10452.05000000001</v>
       </c>
       <c r="D100" s="12">
-        <v>1.573277238289261E-4</v>
+        <v>1.952151241961797E-4</v>
       </c>
       <c r="E100">
         <v>-0.18627250506907489</v>
@@ -3432,16 +3445,16 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101" s="11">
-        <v>99</v>
+        <v>32</v>
       </c>
       <c r="B101" s="6">
-        <v>44943.624537037038</v>
+        <v>44929.790277777778</v>
       </c>
       <c r="C101" s="1">
-        <v>10817.72000000001</v>
+        <v>10411.33</v>
       </c>
       <c r="D101" s="12">
-        <v>9.7620376102147688E-4</v>
+        <v>1.959787843359706E-4</v>
       </c>
       <c r="E101">
         <v>-0.18627250506907489</v>
@@ -3458,16 +3471,16 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102" s="11">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="B102" s="6">
-        <v>44943.862500000003</v>
+        <v>44951.512499999997</v>
       </c>
       <c r="C102" s="1">
-        <v>10818.77000000001</v>
+        <v>10375.69</v>
       </c>
       <c r="D102" s="12">
-        <v>9.7062967057581773E-5</v>
+        <v>2.1497166808370771E-4</v>
       </c>
       <c r="E102">
         <v>-0.18627250506907489</v>
@@ -3484,16 +3497,16 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103" s="11">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="B103" s="6">
-        <v>44944.280578703707</v>
+        <v>44930.421134259261</v>
       </c>
       <c r="C103" s="1">
-        <v>10801.400000000011</v>
+        <v>10381.69000000001</v>
       </c>
       <c r="D103" s="12">
-        <v>-1.6055429591349531E-3</v>
+        <v>2.2062932346766931E-4</v>
       </c>
       <c r="E103">
         <v>-0.18627250506907489</v>
@@ -3510,16 +3523,16 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" s="11">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="B104" s="6">
-        <v>44944.375439814823</v>
+        <v>44944.195844907408</v>
       </c>
       <c r="C104" s="1">
-        <v>10785.160000000011</v>
+        <v>10373.459999999999</v>
       </c>
       <c r="D104" s="12">
-        <v>-1.5035088044141891E-3</v>
+        <v>2.2466211492866431E-4</v>
       </c>
       <c r="E104">
         <v>-0.18627250506907489</v>
@@ -3536,16 +3549,16 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105" s="11">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="B105" s="6">
-        <v>44944.388553240737</v>
+        <v>44931.714629629627</v>
       </c>
       <c r="C105" s="1">
-        <v>10773.510000000009</v>
+        <v>10448.19000000001</v>
       </c>
       <c r="D105" s="12">
-        <v>-1.0801879619773971E-3</v>
+        <v>2.3550292799057179E-4</v>
       </c>
       <c r="E105">
         <v>-0.18627250506907489</v>
@@ -3562,16 +3575,16 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106" s="11">
-        <v>104</v>
+        <v>2</v>
       </c>
       <c r="B106" s="6">
-        <v>44944.406585648147</v>
+        <v>44928.388865740737</v>
       </c>
       <c r="C106" s="1">
-        <v>10772.64</v>
+        <v>10340.290000000001</v>
       </c>
       <c r="D106" s="12">
-        <v>-8.0753626255591904E-5</v>
+        <v>2.6021513697571658E-4</v>
       </c>
       <c r="E106">
         <v>-0.18627250506907489</v>
@@ -3588,16 +3601,16 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107" s="11">
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="B107" s="6">
-        <v>44944.470173611109</v>
+        <v>44953.450243055559</v>
       </c>
       <c r="C107" s="1">
-        <v>10786.61</v>
+        <v>10920.13</v>
       </c>
       <c r="D107" s="12">
-        <v>1.296803754696985E-3</v>
+        <v>4.6357925327078497E-4</v>
       </c>
       <c r="E107">
         <v>-0.18627250506907489</v>
@@ -3614,16 +3627,16 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="11">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="B108" s="6">
-        <v>44944.471192129633</v>
+        <v>44951.851493055547</v>
       </c>
       <c r="C108" s="1">
-        <v>10799.22</v>
+        <v>10909</v>
       </c>
       <c r="D108" s="12">
-        <v>1.1690419881686951E-3</v>
+        <v>4.6680502682061592E-4</v>
       </c>
       <c r="E108">
         <v>-0.18627250506907489</v>
@@ -3640,16 +3653,16 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109" s="11">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="B109" s="6">
-        <v>44944.49114583333</v>
+        <v>44950.15415509259</v>
       </c>
       <c r="C109" s="1">
-        <v>10816.12</v>
+        <v>10880.93</v>
       </c>
       <c r="D109" s="12">
-        <v>1.5649278373808251E-3</v>
+        <v>4.6800982728689711E-4</v>
       </c>
       <c r="E109">
         <v>-0.18627250506907489</v>
@@ -3666,16 +3679,16 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110" s="11">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B110" s="6">
-        <v>44944.499594907407</v>
+        <v>44943.428611111107</v>
       </c>
       <c r="C110" s="1">
-        <v>10833.48000000001</v>
+        <v>10808.04000000001</v>
       </c>
       <c r="D110" s="12">
-        <v>1.605011778715415E-3</v>
+        <v>4.6838927777326228E-4</v>
       </c>
       <c r="E110">
         <v>-0.18627250506907489</v>
@@ -3692,16 +3705,16 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111" s="11">
-        <v>109</v>
+        <v>142</v>
       </c>
       <c r="B111" s="6">
-        <v>44944.630555555559</v>
+        <v>44952.863344907397</v>
       </c>
       <c r="C111" s="1">
-        <v>10830.77000000001</v>
+        <v>10915.46</v>
       </c>
       <c r="D111" s="12">
-        <v>-2.5015045950138592E-4</v>
+        <v>4.6927960081921682E-4</v>
       </c>
       <c r="E111">
         <v>-0.18627250506907489</v>
@@ -3718,16 +3731,16 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112" s="11">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="B112" s="6">
-        <v>44944.645914351851</v>
+        <v>44931.434976851851</v>
       </c>
       <c r="C112" s="1">
-        <v>10831.930000000009</v>
+        <v>10441.87000000001</v>
       </c>
       <c r="D112" s="12">
-        <v>1.071022651206732E-4</v>
+        <v>4.8769831308126399E-4</v>
       </c>
       <c r="E112">
         <v>-0.18627250506907489</v>
@@ -3744,16 +3757,16 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="11">
-        <v>111</v>
+        <v>43</v>
       </c>
       <c r="B113" s="6">
-        <v>44944.677199074067</v>
+        <v>44931.104166666657</v>
       </c>
       <c r="C113" s="1">
-        <v>10840.04000000001</v>
+        <v>10435.14000000001</v>
       </c>
       <c r="D113" s="12">
-        <v>7.4871237166429516E-4</v>
+        <v>4.9089071737173917E-4</v>
       </c>
       <c r="E113">
         <v>-0.18627250506907489</v>
@@ -3770,16 +3783,16 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114" s="11">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="B114" s="6">
-        <v>44944.789629629631</v>
+        <v>44942.51085648148</v>
       </c>
       <c r="C114" s="1">
-        <v>10841.910000000011</v>
+        <v>10801.36000000001</v>
       </c>
       <c r="D114" s="12">
-        <v>1.72508588529352E-4</v>
+        <v>4.9091983556959207E-4</v>
       </c>
       <c r="E114">
         <v>-0.18627250506907489</v>
@@ -3796,16 +3809,16 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115" s="11">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="B115" s="6">
-        <v>44944.915972222218</v>
+        <v>44929.258506944447</v>
       </c>
       <c r="C115" s="1">
-        <v>10843.820000000011</v>
+        <v>10400.51</v>
       </c>
       <c r="D115" s="12">
-        <v>1.7616822128196929E-4</v>
+        <v>4.9541333825864342E-4</v>
       </c>
       <c r="E115">
         <v>-0.18627250506907489</v>
@@ -3822,42 +3835,42 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116" s="11">
-        <v>114</v>
+        <v>18</v>
       </c>
       <c r="B116" s="6">
-        <v>44945.1875</v>
+        <v>44925.796932870369</v>
       </c>
       <c r="C116" s="1">
-        <v>10840.71000000001</v>
+        <v>10382.379999999999</v>
       </c>
       <c r="D116" s="12">
-        <v>-2.867993013532244E-4</v>
+        <v>4.9627887210745847E-4</v>
       </c>
       <c r="E116">
         <v>-0.18627250506907489</v>
       </c>
       <c r="F116" s="2">
-        <v>4.4385392570033273E-2</v>
+        <v>4.6060746222620352E-4</v>
       </c>
       <c r="G116" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H116" s="5">
-        <v>0.17754157028013309</v>
+        <v>1.8424298489048141E-3</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117" s="11">
-        <v>115</v>
+        <v>13</v>
       </c>
       <c r="B117" s="6">
-        <v>44945.403217592589</v>
+        <v>44937.147349537037</v>
       </c>
       <c r="C117" s="1">
-        <v>10841.750000000009</v>
+        <v>10371.129999999999</v>
       </c>
       <c r="D117" s="12">
-        <v>9.593467586532789E-5</v>
+        <v>5.112952846033636E-4</v>
       </c>
       <c r="E117">
         <v>-0.18627250506907489</v>
@@ -3874,16 +3887,16 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118" s="11">
-        <v>116</v>
+        <v>22</v>
       </c>
       <c r="B118" s="6">
-        <v>44945.486643518518</v>
+        <v>44929.044699074067</v>
       </c>
       <c r="C118" s="1">
-        <v>10851.580000000011</v>
+        <v>10391.950000000001</v>
       </c>
       <c r="D118" s="12">
-        <v>9.0668019461803695E-4</v>
+        <v>5.6228944234182343E-4</v>
       </c>
       <c r="E118">
         <v>-0.18627250506907489</v>
@@ -3900,16 +3913,16 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119" s="11">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="B119" s="6">
-        <v>44945.688194444447</v>
+        <v>44932.645925925928</v>
       </c>
       <c r="C119" s="1">
-        <v>10853.570000000011</v>
+        <v>10463.500000000009</v>
       </c>
       <c r="D119" s="12">
-        <v>1.8338343356449899E-4</v>
+        <v>5.9575778381915079E-4</v>
       </c>
       <c r="E119">
         <v>-0.18627250506907489</v>
@@ -3926,16 +3939,16 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120" s="11">
-        <v>118</v>
+        <v>30</v>
       </c>
       <c r="B120" s="6">
-        <v>44945.773622685178</v>
+        <v>44929.67564814815</v>
       </c>
       <c r="C120" s="1">
-        <v>10850.660000000011</v>
+        <v>10400.9</v>
       </c>
       <c r="D120" s="12">
-        <v>-2.6811454664221751E-4</v>
+        <v>6.7636020077221914E-4</v>
       </c>
       <c r="E120">
         <v>-0.18627250506907489</v>
@@ -3952,16 +3965,16 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121" s="11">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B121" s="6">
-        <v>44945.797488425917</v>
+        <v>44944.677199074067</v>
       </c>
       <c r="C121" s="1">
-        <v>10852.30000000001</v>
+        <v>10840.04000000001</v>
       </c>
       <c r="D121" s="12">
-        <v>1.5114287978801319E-4</v>
+        <v>7.4871237166429516E-4</v>
       </c>
       <c r="E121">
         <v>-0.18627250506907489</v>
@@ -3978,16 +3991,16 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122" s="11">
-        <v>120</v>
+        <v>31</v>
       </c>
       <c r="B122" s="6">
-        <v>44946.096493055556</v>
+        <v>44929.695497685178</v>
       </c>
       <c r="C122" s="1">
-        <v>10862.13000000001</v>
+        <v>10409.290000000001</v>
       </c>
       <c r="D122" s="12">
-        <v>9.0579877076746307E-4</v>
+        <v>8.0666096203207971E-4</v>
       </c>
       <c r="E122">
         <v>-0.18627250506907489</v>
@@ -4004,42 +4017,42 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="11">
-        <v>121</v>
+        <v>151</v>
       </c>
       <c r="B123" s="6">
-        <v>44949.086111111108</v>
+        <v>44956.504930555559</v>
       </c>
       <c r="C123" s="1">
-        <v>10859.100000000009</v>
+        <v>10936.18</v>
       </c>
       <c r="D123" s="12">
-        <v>-2.7895081351458911E-4</v>
+        <v>8.8500353726850278E-4</v>
       </c>
       <c r="E123">
         <v>-0.18627250506907489</v>
       </c>
-      <c r="F123" s="2">
+      <c r="F123">
         <v>4.4385392570033273E-2</v>
       </c>
       <c r="G123" t="s">
         <v>15</v>
       </c>
-      <c r="H123" s="5">
+      <c r="H123">
         <v>0.17754157028013309</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="11">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B124" s="6">
-        <v>44949.135416666657</v>
+        <v>44951.348796296297</v>
       </c>
       <c r="C124" s="1">
-        <v>10860.350000000009</v>
+        <v>10893.51</v>
       </c>
       <c r="D124" s="12">
-        <v>1.151108287058555E-4</v>
+        <v>8.9583011753280317E-4</v>
       </c>
       <c r="E124">
         <v>-0.18627250506907489</v>
@@ -4056,16 +4069,16 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="11">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B125" s="6">
-        <v>44949.36991898148</v>
+        <v>44946.096493055556</v>
       </c>
       <c r="C125" s="1">
-        <v>10870.500000000009</v>
+        <v>10862.13000000001</v>
       </c>
       <c r="D125" s="12">
-        <v>9.3459234739201591E-4</v>
+        <v>9.0579877076746307E-4</v>
       </c>
       <c r="E125">
         <v>-0.18627250506907489</v>
@@ -4082,16 +4095,16 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126" s="11">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B126" s="6">
-        <v>44949.615972222222</v>
+        <v>44945.486643518518</v>
       </c>
       <c r="C126" s="1">
-        <v>10872.31</v>
+        <v>10851.580000000011</v>
       </c>
       <c r="D126" s="12">
-        <v>1.665056805113529E-4</v>
+        <v>9.0668019461803695E-4</v>
       </c>
       <c r="E126">
         <v>-0.18627250506907489</v>
@@ -4108,16 +4121,16 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127" s="11">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="B127" s="6">
-        <v>44949.700023148151</v>
+        <v>44951.711296296293</v>
       </c>
       <c r="C127" s="1">
-        <v>10874.36</v>
+        <v>10904.32</v>
       </c>
       <c r="D127" s="12">
-        <v>1.8855238675130609E-4</v>
+        <v>9.3169098701406661E-4</v>
       </c>
       <c r="E127">
         <v>-0.18627250506907489</v>
@@ -4134,16 +4147,16 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128" s="11">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B128" s="6">
-        <v>44949.729884259257</v>
+        <v>44949.36991898148</v>
       </c>
       <c r="C128" s="1">
-        <v>10876.21</v>
+        <v>10870.500000000009</v>
       </c>
       <c r="D128" s="12">
-        <v>1.7012495448009979E-4</v>
+        <v>9.3459234739201591E-4</v>
       </c>
       <c r="E128">
         <v>-0.18627250506907489</v>
@@ -4160,16 +4173,16 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129" s="11">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="B129" s="6">
-        <v>44949.918749999997</v>
+        <v>44938.836238425924</v>
       </c>
       <c r="C129" s="1">
-        <v>10875.84</v>
+        <v>10790.56000000001</v>
       </c>
       <c r="D129" s="12">
-        <v>-3.4019203380641898E-5</v>
+        <v>9.6380669321538548E-4</v>
       </c>
       <c r="E129">
         <v>-0.18627250506907489</v>
@@ -4186,16 +4199,16 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="11">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="B130" s="6">
-        <v>44950.15415509259</v>
+        <v>44943.624537037038</v>
       </c>
       <c r="C130" s="1">
-        <v>10880.93</v>
+        <v>10817.72000000001</v>
       </c>
       <c r="D130" s="12">
-        <v>4.6800982728689711E-4</v>
+        <v>9.7620376102147688E-4</v>
       </c>
       <c r="E130">
         <v>-0.18627250506907489</v>
@@ -4212,16 +4225,16 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131" s="11">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="B131" s="6">
-        <v>44950.526400462957</v>
+        <v>44928.414560185192</v>
       </c>
       <c r="C131" s="1">
-        <v>10882.76</v>
+        <v>10350.56</v>
       </c>
       <c r="D131" s="12">
-        <v>1.6818415337649381E-4</v>
+        <v>9.9320231831034889E-4</v>
       </c>
       <c r="E131">
         <v>-0.18627250506907489</v>
@@ -4238,16 +4251,16 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132" s="11">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="B132" s="6">
-        <v>44950.554907407408</v>
+        <v>44944.471192129633</v>
       </c>
       <c r="C132" s="1">
-        <v>10884.73</v>
+        <v>10799.22</v>
       </c>
       <c r="D132" s="12">
-        <v>1.810202558909513E-4</v>
+        <v>1.1690419881686951E-3</v>
       </c>
       <c r="E132">
         <v>-0.18627250506907489</v>
@@ -4264,16 +4277,16 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133" s="11">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="B133" s="6">
-        <v>44950.740300925929</v>
+        <v>44929.459849537037</v>
       </c>
       <c r="C133" s="1">
-        <v>10882</v>
+        <v>10318.93</v>
       </c>
       <c r="D133" s="12">
-        <v>-2.5081007980898301E-4</v>
+        <v>1.255580492509845E-3</v>
       </c>
       <c r="E133">
         <v>-0.18627250506907489</v>
@@ -4290,16 +4303,16 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134" s="11">
-        <v>132</v>
+        <v>37</v>
       </c>
       <c r="B134" s="6">
-        <v>44951.082870370366</v>
+        <v>44930.427187499998</v>
       </c>
       <c r="C134" s="1">
-        <v>10883.76</v>
+        <v>10394.79000000001</v>
       </c>
       <c r="D134" s="12">
-        <v>1.6173497518834351E-4</v>
+        <v>1.2618369456225409E-3</v>
       </c>
       <c r="E134">
         <v>-0.18627250506907489</v>
@@ -4316,16 +4329,16 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135" s="11">
-        <v>133</v>
+        <v>105</v>
       </c>
       <c r="B135" s="6">
-        <v>44951.348796296297</v>
+        <v>44944.470173611109</v>
       </c>
       <c r="C135" s="1">
-        <v>10893.51</v>
+        <v>10786.61</v>
       </c>
       <c r="D135" s="12">
-        <v>8.9583011753280317E-4</v>
+        <v>1.296803754696985E-3</v>
       </c>
       <c r="E135">
         <v>-0.18627250506907489</v>
@@ -4342,16 +4355,16 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136" s="11">
-        <v>134</v>
+        <v>38</v>
       </c>
       <c r="B136" s="6">
-        <v>44951.480567129627</v>
+        <v>44930.43822916667</v>
       </c>
       <c r="C136" s="1">
-        <v>10895.36</v>
+        <v>10408.400000000011</v>
       </c>
       <c r="D136" s="12">
-        <v>1.6982588715674929E-4</v>
+        <v>1.309309759985666E-3</v>
       </c>
       <c r="E136">
         <v>-0.18627250506907489</v>
@@ -4368,16 +4381,16 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A137" s="11">
-        <v>135</v>
+        <v>10</v>
       </c>
       <c r="B137" s="6">
-        <v>44951.617361111108</v>
+        <v>44929.517858796287</v>
       </c>
       <c r="C137" s="1">
-        <v>10892.41</v>
+        <v>10347.84</v>
       </c>
       <c r="D137" s="12">
-        <v>-2.7075746005644769E-4</v>
+        <v>1.383843290876152E-3</v>
       </c>
       <c r="E137">
         <v>-0.18627250506907489</v>
@@ -4394,16 +4407,16 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A138" s="11">
-        <v>136</v>
+        <v>9</v>
       </c>
       <c r="B138" s="6">
-        <v>44951.695104166669</v>
+        <v>44929.461782407408</v>
       </c>
       <c r="C138" s="1">
-        <v>10894.17</v>
+        <v>10333.540000000001</v>
       </c>
       <c r="D138" s="12">
-        <v>1.615804032348844E-4</v>
+        <v>1.4158444722467409E-3</v>
       </c>
       <c r="E138">
         <v>-0.18627250506907489</v>
@@ -4420,16 +4433,16 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A139" s="11">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="B139" s="6">
-        <v>44951.711296296293</v>
+        <v>44944.49114583333</v>
       </c>
       <c r="C139" s="1">
-        <v>10904.32</v>
+        <v>10816.12</v>
       </c>
       <c r="D139" s="12">
-        <v>9.3169098701406661E-4</v>
+        <v>1.5649278373808251E-3</v>
       </c>
       <c r="E139">
         <v>-0.18627250506907489</v>
@@ -4446,16 +4459,16 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="11">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="B140" s="6">
-        <v>44951.787546296298</v>
+        <v>44944.499594907407</v>
       </c>
       <c r="C140" s="1">
-        <v>10903.91</v>
+        <v>10833.48000000001</v>
       </c>
       <c r="D140" s="12">
-        <v>-3.7599776969154952E-5</v>
+        <v>1.605011778715415E-3</v>
       </c>
       <c r="E140">
         <v>-0.18627250506907489</v>
@@ -4472,16 +4485,16 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A141" s="11">
-        <v>139</v>
+        <v>11</v>
       </c>
       <c r="B141" s="6">
-        <v>44951.851493055547</v>
+        <v>44929.555300925917</v>
       </c>
       <c r="C141" s="1">
-        <v>10909</v>
+        <v>10366.299999999999</v>
       </c>
       <c r="D141" s="12">
-        <v>4.6680502682061592E-4</v>
+        <v>1.7839471812473029E-3</v>
       </c>
       <c r="E141">
         <v>-0.18627250506907489</v>
@@ -4498,16 +4511,16 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A142" s="11">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="B142" s="6">
-        <v>44952.524305555547</v>
+        <v>44930.47928240741</v>
       </c>
       <c r="C142" s="1">
-        <v>10910.81</v>
+        <v>10427.420000000009</v>
       </c>
       <c r="D142" s="12">
-        <v>1.6591804931698209E-4</v>
+        <v>1.827370200991441E-3</v>
       </c>
       <c r="E142">
         <v>-0.18627250506907489</v>
@@ -4524,16 +4537,16 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A143" s="11">
-        <v>141</v>
+        <v>67</v>
       </c>
       <c r="B143" s="6">
-        <v>44952.828472222223</v>
+        <v>44935.151863425926</v>
       </c>
       <c r="C143" s="1">
-        <v>10910.34</v>
+        <v>9363.0500000000084</v>
       </c>
       <c r="D143" s="12">
-        <v>-4.307654518764803E-5</v>
+        <v>2.9747366977745941E-3</v>
       </c>
       <c r="E143">
         <v>-0.18627250506907489</v>
@@ -4550,16 +4563,16 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A144" s="11">
-        <v>142</v>
+        <v>70</v>
       </c>
       <c r="B144" s="6">
-        <v>44952.863344907397</v>
+        <v>44935.720451388886</v>
       </c>
       <c r="C144" s="1">
-        <v>10915.46</v>
+        <v>8823.2700000000077</v>
       </c>
       <c r="D144" s="12">
-        <v>4.6927960081921682E-4</v>
+        <v>6.42068306303889E-3</v>
       </c>
       <c r="E144">
         <v>-0.18627250506907489</v>
@@ -4576,16 +4589,16 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A145" s="11">
-        <v>143</v>
+        <v>71</v>
       </c>
       <c r="B145" s="6">
-        <v>44953.313888888893</v>
+        <v>44935.72420138889</v>
       </c>
       <c r="C145" s="1">
-        <v>10915.070000000011</v>
+        <v>8887.7700000000077</v>
       </c>
       <c r="D145" s="12">
-        <v>-3.572914013694195E-5</v>
+        <v>7.3102149203185807E-3</v>
       </c>
       <c r="E145">
         <v>-0.18627250506907489</v>
@@ -4602,16 +4615,16 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A146" s="11">
-        <v>144</v>
+        <v>72</v>
       </c>
       <c r="B146" s="6">
-        <v>44953.450243055559</v>
+        <v>44936.094629629632</v>
       </c>
       <c r="C146" s="1">
-        <v>10920.13</v>
+        <v>8955.6300000000083</v>
       </c>
       <c r="D146" s="12">
-        <v>4.6357925327078497E-4</v>
+        <v>7.6352110821951147E-3</v>
       </c>
       <c r="E146">
         <v>-0.18627250506907489</v>
@@ -4628,16 +4641,16 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A147" s="11">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="B147" s="6">
-        <v>44953.647245370368</v>
+        <v>44937.47047453704</v>
       </c>
       <c r="C147" s="1">
-        <v>10922.02</v>
+        <v>9413.820000000007</v>
       </c>
       <c r="D147" s="12">
-        <v>1.7307486266182609E-4</v>
+        <v>1.189814610781537E-2</v>
       </c>
       <c r="E147">
         <v>-0.18627250506907489</v>
@@ -4654,16 +4667,16 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="11">
-        <v>146</v>
+        <v>74</v>
       </c>
       <c r="B148" s="6">
-        <v>44953.696539351848</v>
+        <v>44936.667129629634</v>
       </c>
       <c r="C148" s="1">
-        <v>10924.01</v>
+        <v>8924.6600000000089</v>
       </c>
       <c r="D148" s="12">
-        <v>1.822007284366656E-4</v>
+        <v>1.213818225532259E-2</v>
       </c>
       <c r="E148">
         <v>-0.18627250506907489</v>
@@ -4680,16 +4693,16 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="11">
-        <v>147</v>
+        <v>76</v>
       </c>
       <c r="B149" s="6">
-        <v>44956.059178240743</v>
+        <v>44936.818287037036</v>
       </c>
       <c r="C149" s="1">
-        <v>10925.9</v>
+        <v>8656.4600000000082</v>
       </c>
       <c r="D149" s="12">
-        <v>1.7301338977171449E-4</v>
+        <v>1.6493658994833241E-2</v>
       </c>
       <c r="E149">
         <v>-0.18627250506907489</v>
@@ -4706,16 +4719,16 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A150" s="11">
-        <v>148</v>
+        <v>78</v>
       </c>
       <c r="B150" s="6">
-        <v>44956.379166666673</v>
+        <v>44937.317881944437</v>
       </c>
       <c r="C150" s="1">
-        <v>10927.77</v>
+        <v>8803.6700000000073</v>
       </c>
       <c r="D150" s="12">
-        <v>1.7115294849867621E-4</v>
+        <v>2.3036617577506299E-2</v>
       </c>
       <c r="E150">
         <v>-0.18627250506907489</v>
@@ -4732,16 +4745,16 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="11">
-        <v>149</v>
+        <v>79</v>
       </c>
       <c r="B151" s="6">
-        <v>44956.417372685188</v>
+        <v>44937.421574074076</v>
       </c>
       <c r="C151" s="1">
-        <v>10924.78</v>
+        <v>9043.9000000000069</v>
       </c>
       <c r="D151" s="12">
-        <v>-2.7361483632981631E-4</v>
+        <v>2.7287483515397559E-2</v>
       </c>
       <c r="E151">
         <v>-0.18627250506907489</v>
@@ -4758,16 +4771,16 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="11">
-        <v>150</v>
+        <v>80</v>
       </c>
       <c r="B152" s="6">
-        <v>44956.475578703707</v>
+        <v>44937.444606481477</v>
       </c>
       <c r="C152" s="1">
-        <v>10926.51</v>
+        <v>9303.1300000000065</v>
       </c>
       <c r="D152" s="12">
-        <v>1.5835559160004559E-4</v>
+        <v>2.8663519057043899E-2</v>
       </c>
       <c r="E152">
         <v>-0.18627250506907489</v>
@@ -4784,42 +4797,42 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="11">
-        <v>151</v>
+        <v>82</v>
       </c>
       <c r="B153" s="6">
-        <v>44956.504930555559</v>
+        <v>44937.472256944442</v>
       </c>
       <c r="C153" s="1">
-        <v>10936.18</v>
+        <v>9690.8700000000063</v>
       </c>
       <c r="D153" s="12">
-        <v>8.8500353726850278E-4</v>
+        <v>2.9430135694117791E-2</v>
       </c>
       <c r="E153">
         <v>-0.18627250506907489</v>
       </c>
-      <c r="F153">
+      <c r="F153" s="2">
         <v>4.4385392570033273E-2</v>
       </c>
       <c r="G153" t="s">
         <v>15</v>
       </c>
-      <c r="H153">
+      <c r="H153" s="5">
         <v>0.17754157028013309</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="11">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="B154" s="6">
-        <v>44956.690983796303</v>
+        <v>44937.573206018518</v>
       </c>
       <c r="C154" s="1">
-        <v>10938.09</v>
+        <v>10023.55000000001</v>
       </c>
       <c r="D154" s="12">
-        <v>1.7464964914615239E-4</v>
+        <v>3.4329219151634449E-2</v>
       </c>
       <c r="E154">
         <v>-0.18627250506907489</v>
@@ -4836,16 +4849,16 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="11">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="B155" s="6">
-        <v>44956.916678240741</v>
+        <v>44937.678206018521</v>
       </c>
       <c r="C155" s="1">
-        <v>10939.96</v>
+        <v>10388.330000000011</v>
       </c>
       <c r="D155" s="12">
-        <v>1.7096220638168619E-4</v>
+        <v>3.6392296142584213E-2</v>
       </c>
       <c r="E155">
         <v>-0.18627250506907489</v>
@@ -4862,16 +4875,16 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="11">
-        <v>154</v>
+        <v>85</v>
       </c>
       <c r="B156" s="6">
-        <v>44957.365972222222</v>
+        <v>44937.700902777768</v>
       </c>
       <c r="C156" s="1">
-        <v>10803.01</v>
+        <v>10781.660000000011</v>
       </c>
       <c r="D156" s="12">
-        <v>-1.2518327306498491E-2</v>
+        <v>3.7862678601854112E-2</v>
       </c>
       <c r="E156">
         <v>-0.18627250506907489</v>
@@ -5621,7 +5634,11 @@
       <c r="C296" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H238" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:H238" xr:uid="{00000000-0009-0000-0000-000001000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H238">
+      <sortCondition ref="D1:D238"/>
+    </sortState>
+  </autoFilter>
   <conditionalFormatting sqref="L3:L173">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>

</xml_diff>